<commit_message>
update spec do an
</commit_message>
<xml_diff>
--- a/Report/do an.xlsx
+++ b/Report/do an.xlsx
@@ -12,7 +12,7 @@
     <sheet state="visible" name="Estimate" sheetId="7" r:id="rId10"/>
     <sheet state="visible" name="Sheet3" sheetId="8" r:id="rId11"/>
     <sheet state="visible" name="Sheet4" sheetId="9" r:id="rId12"/>
-    <sheet state="visible" name="phí đóng gói" sheetId="10" r:id="rId13"/>
+    <sheet state="visible" name="msg" sheetId="10" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName hidden="1" localSheetId="6" name="_xlnm._FilterDatabase">Estimate!$A$1:$E$32</definedName>
@@ -20,14 +20,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId14" roundtripDataChecksum="78WcQWzp+D3WakRCXwqvaTKxQ7mTrPe0tJYCj983S+8="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId14" roundtripDataChecksum="V6SNANVit/Q3hY9fEi5KzOUlYY9DTk4W/VD50w2rCoM="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="566">
   <si>
     <t>Nhập: số tầng, loại nhà, diện tích và số phòng</t>
   </si>
@@ -2605,10 +2605,97 @@
     <t>toàn bộ 5tr cọc trước 2tr (đã bao gồm phí di chuyển review)</t>
   </si>
   <si>
+    <t>As the MoveMate system administrator,</t>
+  </si>
+  <si>
+    <t>I want to manage the active moving bookings so that I can track the overall status and progress of each booking.</t>
+  </si>
+  <si>
+    <t>I want to manage the available drivers and porters so that I can assign jobs efficiently and ensure enough personnel are available to handle bookings.</t>
+  </si>
+  <si>
+    <t>I want to manage the vehicle fleet so that I can keep track of vehicle availability, usage, and maintenance schedules.</t>
+  </si>
+  <si>
+    <t>I want to manage customer reviews and feedback so that I can monitor service quality and resolve any issues that arise.</t>
+  </si>
+  <si>
+    <t>I want to manage the payment system so that I can ensure transactions are processed accurately and securely, including deposits and final payments for each move.</t>
+  </si>
+  <si>
+    <t>As a customer,</t>
+  </si>
+  <si>
+    <t>I want to book a moving service so that I can easily schedule my move, select the right vehicle, and specify any additional services like loading or unloading.</t>
+  </si>
+  <si>
+    <t>I want to manage my booking so that I can make changes or cancel my reservation if my plans change.</t>
+  </si>
+  <si>
+    <t>I want to track the progress of my move in real time so that I can be informed about when the driver and porters will arrive.</t>
+  </si>
+  <si>
+    <t>I want to pay for my moving service online so that I can complete the transaction securely and conveniently without needing cash on hand.</t>
+  </si>
+  <si>
+    <t>I want to manage customer inquiries so that I can resolve issues related to booking, payment, or moving services.</t>
+  </si>
+  <si>
+    <t>I want to provide updates to customers regarding their move so that I can keep them informed about any delays or changes.</t>
+  </si>
+  <si>
+    <t>I want to handle complaints and damage claims so that I can resolve any post-move issues and maintain customer satisfaction.</t>
+  </si>
+  <si>
+    <t>I want to see all the cars available so that I can make my choice more easily</t>
+  </si>
+  <si>
+    <t>I want to manage my wallet so that I can keep track of how much I've paid for which services.</t>
+  </si>
+  <si>
+    <t>I want to see information about each service so that I can compare and make a reasonable choice.</t>
+  </si>
+  <si>
+    <t>As a driver,</t>
+  </si>
+  <si>
+    <t>I want to receive assignments so that I know when and where I need to be for each moving job.</t>
+  </si>
+  <si>
+    <t>I want to navigate to the customer’s location with real-time map integration so that I can arrive on time and avoid delays.</t>
+  </si>
+  <si>
+    <t>I want to update the system when I have arrived at the location so that the customer is notified and the job can proceed.</t>
+  </si>
+  <si>
+    <t>I want to confirm the completion of the moving service so that I can ensure the job is logged as finished, and payment can be processed.</t>
+  </si>
+  <si>
+    <t>As a porter,</t>
+  </si>
+  <si>
+    <t>I want to view my assigned jobs so that I can prepare for each move and coordinate with the team.</t>
+  </si>
+  <si>
+    <t>I want to update the system when loading and unloading tasks are completed so that I can ensure accurate reporting of job progress.</t>
+  </si>
+  <si>
+    <t>I want to confirm the completion of my tasks so that the customer knows the service has been completed, and I can log my work hours for payment.</t>
+  </si>
+  <si>
+    <t>Đi theo flow kh chọn ngày giờ, nơi đi và đến  -&gt; upload hình ảnh, video đồ vật -&gt; chọn xe -&gt; chọn dịch vụ -&gt; màn hình xử lý -&gt; deposit -&gt; tracking -&gt; done -&gt; payment</t>
+  </si>
+  <si>
+    <t>xử lý: review có kinh nghiệm xử lý đưa ra cho kh xe dịch vụ hợp lý hơn -&gt; gửi noti cho khách hàng -&gt; màn hình (3 nút: Đồng ý, Hủy, Liên lạc với reviewer qua nhắn gọi điện trong app)</t>
+  </si>
+  <si>
+    <t>trường hợp booking liền</t>
+  </si>
+  <si>
     <t>đổi time</t>
   </si>
   <si>
-    <t>đang tìm</t>
+    <t xml:space="preserve">đang tìm tài xế </t>
   </si>
   <si>
     <t>đã tìm thấy (assign)</t>
@@ -2621,69 +2708,6 @@
   </si>
   <si>
     <t>OK ĐỔI</t>
-  </si>
-  <si>
-    <t>(TH1: review đã review ko trừ)</t>
-  </si>
-  <si>
-    <t>(TH2: CUS DC ĐỔI 1 LẦN khi đã liên lạc dc review)</t>
-  </si>
-  <si>
-    <t>(TH3: ko liên lạc dc vs cus review sẽ có nút update là chờ trong vòng 3 tiếng, sau 3 tiếng ko có phản hồi từ cus sẽ hủy booking và ăn tiền cọc)</t>
-  </si>
-  <si>
-    <t>ko dc đổi trong trường hợp đã review done</t>
-  </si>
-  <si>
-    <t>tình huống trong lúc vận chuyển xảy ra sự cố:</t>
-  </si>
-  <si>
-    <t>1. lỗi của driver potter thì phải report từ cus hoặc driver hoặc potter thì sẽ đền bù 70% giá trị của đồ vật</t>
-  </si>
-  <si>
-    <t>2. lỗi cus khi ko chụp đầy đủ hình ảnh  thì khi driver tới nếu chở ko đủ 1 lần sẽ update đi lần 2 hoặc đổi xe</t>
-  </si>
-  <si>
-    <t>hỏi cô làm thế nào để xác thực cái order của customer</t>
-  </si>
-  <si>
-    <t>1. CÓ REVIEW TỚI</t>
-  </si>
-  <si>
-    <t>ƯU</t>
-  </si>
-  <si>
-    <t>XÁC THỰC CAO, CONNECT TRỰC TIẾP CUS, LINH HOẠT SETTING</t>
-  </si>
-  <si>
-    <t>NHƯỢC</t>
-  </si>
-  <si>
-    <t>TỐN TIME, TỐN RESOURCE</t>
-  </si>
-  <si>
-    <t>2. REVIEW QUA ẢNH VIDEO CUS CUNG CẤP</t>
-  </si>
-  <si>
-    <t>ÍT TỐN RESOURCE, USER KO CẦN ĐỢI REVIEW -&gt; BƯỚC XE TỚI, GIẢM THIỂU THỜI GIAN CUS TẬP TRUNG VÀO 1 BOOKING</t>
-  </si>
-  <si>
-    <t>KO XÁC THỰC, CHƯA CHẮC CONNECT 24/7 CUS PHẢI ĐỢI REVIEW ACCEPT</t>
-  </si>
-  <si>
-    <t>duyệt -&gt; update -&gt; cho user confirm -&gt; nếu ko ok thì mới chat mới alo</t>
-  </si>
-  <si>
-    <t>Đi theo flow kh chọn ngày giờ, nơi đi và đến  -&gt; upload hình ảnh, video đồ vật -&gt; chọn xe -&gt; chọn dịch vụ -&gt; màn hình xử lý -&gt; deposit -&gt; tracking -&gt; done -&gt; payment</t>
-  </si>
-  <si>
-    <t>xử lý: review có kinh nghiệm xử lý đưa ra cho kh xe dịch vụ hợp lý hơn -&gt; gửi noti cho khách hàng -&gt; màn hình (3 nút: Đồng ý, Hủy, Liên lạc với reviewer qua nhắn gọi điện trong app)</t>
-  </si>
-  <si>
-    <t>trường hợp booking liền</t>
-  </si>
-  <si>
-    <t xml:space="preserve">đang tìm tài xế </t>
   </si>
   <si>
     <t>đổi ngày 1 lần miễn phí nhưng phải do driver hoặc potter ở đó report</t>
@@ -2786,10 +2810,30 @@
     <t>Nếu ngoài giờ: Thêm khoản phí ngoài giờ % vào tổng phí.</t>
   </si>
   <si>
-    <t>Phí Đóng Gói</t>
-  </si>
-  <si>
-    <t>Chi Phí Đóng Gói Cơ Bản</t>
+    <t>Dịch vụ bốc xếp đã bao gồm vật tư đóng gói và bao bọc 200.000đ đồng thời hỗ trợ sử dụng dụng cụ bốc vác</t>
+  </si>
+  <si>
+    <t>Phân loại dịch vụ</t>
+  </si>
+  <si>
+    <t>Mô tả</t>
+  </si>
+  <si>
+    <t>Loại dịch vụ</t>
+  </si>
+  <si>
+    <t>Bốc xếp (Bởi tài xế)</t>
+  </si>
+  <si>
+    <t>Phí cơ bản: 120.000đ/người/xe cho tối đa 3 tầng.
+Tăng giá theo tầng: Nếu công trình có 4 đến 5 tầng, giá sẽ tăng thêm 20% cho mỗi tầng. Với công trình trên 5 tầng, giá sẽ tăng thêm 25%.
+Bao gồm: Hỗ trợ bốc xếp hàng hóa bởi tài xế, không bao gồm nhân viên bốc xếp chuyên nghiệp.</t>
+  </si>
+  <si>
+    <t>Bốc xếp</t>
+  </si>
+  <si>
+    <t>120.000đ/người/xe/ 3 tầng</t>
   </si>
   <si>
     <r>
@@ -2799,7 +2843,7 @@
         <color theme="1"/>
         <sz val="11.0"/>
       </rPr>
-      <t>Đóng Gói Hộp Thông Thường:</t>
+      <t>4 đến 5 tầng</t>
     </r>
     <r>
       <rPr>
@@ -2808,8 +2852,11 @@
         <color theme="1"/>
         <sz val="11.0"/>
       </rPr>
-      <t xml:space="preserve"> Đóng gói các vật dụng nhỏ trong hộp carton.</t>
+      <t>: Tăng giá thêm 20% cho mỗi tầng.</t>
     </r>
+  </si>
+  <si>
+    <t>400.000đ/người/ 3 tầng</t>
   </si>
   <si>
     <r>
@@ -2817,260 +2864,329 @@
         <rFont val="Calibri"/>
         <b/>
         <color theme="1"/>
-        <sz val="11.0"/>
       </rPr>
-      <t>Giá tham khảo:</t>
+      <t xml:space="preserve">+5 tầng: </t>
     </r>
     <r>
       <rPr>
         <rFont val="Calibri"/>
         <b val="0"/>
         <color theme="1"/>
-        <sz val="11.0"/>
       </rPr>
-      <t xml:space="preserve"> 10,000 VND/hộp</t>
+      <t>25%</t>
     </r>
   </si>
   <si>
-    <t>cho khách chọn mua tùy thích đóng gói xong mới tính giá</t>
-  </si>
-  <si>
-    <t>Chi Phí Đóng Gói Đặc Biệt</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>Đóng Gói Đồ Đạc Cồng Kềnh:</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b val="0"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t xml:space="preserve"> Đóng gói đồ đạc lớn như sofa, tủ lạnh, máy giặt.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>Giá tham khảo:</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b val="0"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t xml:space="preserve"> 200,000 - 500,000 VND/món</t>
-    </r>
-  </si>
-  <si>
-    <t>Chi Phí Đóng Gói Bảo Vệ</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>Đóng Gói Bằng Vật Liệu Bảo Vệ:</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b val="0"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t xml:space="preserve"> Sử dụng bọt khí, xốp, hoặc giấy gói để bảo vệ đồ đạc nhạy cảm.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>Giá tham khảo:</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b val="0"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t xml:space="preserve"> 100,000 - 300,000 VND/m2 hoặc 50,000 - 150,000 VND/món (tùy thuộc vào loại vật liệu)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>Đóng Gói Đồ Nghệ Thuật hoặc Giá Trị Cao:</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b val="0"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t xml:space="preserve"> Đóng gói các món đồ dễ vỡ hoặc có giá trị cao (như tranh, đồ cổ).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>Giá tham khảo:</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b val="0"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t xml:space="preserve"> 300,000 - 600,000 VND/món</t>
-    </r>
-  </si>
-  <si>
-    <t>Chi Phí Đóng Gói Đối Với Hàng Hóa Nhỏ</t>
-  </si>
-  <si>
-    <t>Đóng Gói Hàng Hóa Nhỏ (Như Đồ Điện Tử, Đồ Gia Dụng Nhỏ):</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>Giá tham khảo:</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b val="0"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t xml:space="preserve"> 20,000 - 50,000 VND/món</t>
-    </r>
-  </si>
-  <si>
-    <t>Chi Phí Đóng Gói Hộp Cồng Kềnh</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>Đóng Gói Hộp Lớn hoặc Thùng Cồng Kềnh:</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b val="0"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t xml:space="preserve"> Phí cho việc đóng gói hộp lớn hoặc thùng.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>Giá tham khảo:</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b val="0"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t xml:space="preserve"> 150,000 - 300,000 VND/hộp/thùng</t>
-    </r>
-  </si>
-  <si>
-    <t>Chi Phí Đóng Gói Lại</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>Đóng Gói Lại Các Món Đã Được Đóng Gói Trước:</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b val="0"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t xml:space="preserve"> Nếu cần phải đóng gói lại các món đồ đã được đóng gói trước đó.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>Giá tham khảo:</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b val="0"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t xml:space="preserve"> 100,000 - 200,000 VND/món</t>
-    </r>
+    <t>3 tầng: 50.000đ | 4 - 5 tầng: 100.000đ | +5 tầng: 150.000đ</t>
+  </si>
+  <si>
+    <t>Bốc xếp (Bởi nhân viên bốc xếp)</t>
+  </si>
+  <si>
+    <t>Phí cơ bản: 400.000đ/người cho tối đa 3 tầng.
+Tăng giá theo tầng: Từ 4 đến 5 tầng, giá tăng thêm 20% cho mỗi tầng. Với trên 5 tầng, giá sẽ tăng thêm 25%.
+Bao gồm: Nhân viên bốc xếp chuyên nghiệp đảm bảo hàng hóa được xử lý an toàn và nhanh chóng.</t>
+  </si>
+  <si>
+    <t>50 - 100m: 100.000đ | 100 - 200m: 150.000đ | +200m: 200.000đ</t>
+  </si>
+  <si>
+    <t>190.000đ/người/xe/ 3 tầng</t>
+  </si>
+  <si>
+    <t>470.000đ/người/ 3 tầng</t>
+  </si>
+  <si>
+    <t>Bốc xếp sử dụng thang máy nhỏ hoặc không có thang máy</t>
+  </si>
+  <si>
+    <t>Giá phụ thu theo tầng: 3 tầng: 50.000đ, 4 đến 5 tầng: 100.000đ, trên 5 tầng: 150.000đ.
+Bao gồm: Hỗ trợ di chuyển hàng hóa trong những công trình có thang máy nhỏ hoặc không có thang máy.</t>
+  </si>
+  <si>
+    <t>300.000đ/bộ</t>
+  </si>
+  <si>
+    <t>150.000đ/bộ: đồ vật nhỏ &lt;=5kg | 300.000đ/bộ: đồ vật lớn &gt;6kg</t>
+  </si>
+  <si>
+    <t>Bốc xếp tại địa điểm khó tiếp cận
+50 - 100m: 100.000đ/ người
+100 - 200m: 150.000đ/ người
+trên 200m: 200.000đ/ người</t>
+  </si>
+  <si>
+    <t>Giá phụ thu theo khoảng cách: 50 - 100m: 100.000đ, 100 - 200m: 150.000đ, trên 200m: 200.000đ.
+Bao gồm: Phí này áp dụng cho những địa điểm mà xe tải không thể đến gần, cần di chuyển hàng hóa bằng tay hoặc xe đẩy qua những quãng đường dài.</t>
+  </si>
+  <si>
+    <t>60.000đ/h</t>
+  </si>
+  <si>
+    <t>10.000đ/ng</t>
+  </si>
+  <si>
+    <t>5.000đ</t>
+  </si>
+  <si>
+    <t>Bốc xếp ngoài giờ (Bởi tài xế)</t>
+  </si>
+  <si>
+    <t>Phí cơ bản: 190.000đ/người/xe cho tối đa 3 tầng.
+Tăng giá theo tầng: Nếu công trình có 4 đến 5 tầng, giá sẽ tăng thêm 20% cho mỗi tầng. Với công trình trên 5 tầng, giá sẽ tăng thêm 25%.
+Bao gồm: Hỗ trợ bốc xếp hàng hóa bởi tài xế, không bao gồm nhân viên bốc xếp chuyên nghiệp.</t>
+  </si>
+  <si>
+    <t>Bốc xếp ngoài giờ (Bởi nhân viên bốc xếp)</t>
+  </si>
+  <si>
+    <t>Phí cơ bản: 470.000đ/người cho tối đa 3 tầng.
+Tăng giá theo tầng: Từ 4 đến 5 tầng, giá tăng thêm 20% cho mỗi tầng. Với trên 5 tầng, giá sẽ tăng thêm 25%.
+Bao gồm: Nhân viên bốc xếp chuyên nghiệp đảm bảo hàng hóa được xử lý an toàn và nhanh chóng.</t>
+  </si>
+  <si>
+    <t>Tháo lắp, đóng gói máy lạnh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phí: 300.000đ/bộ.						
+Bao gồm: Dịch vụ tháo lắp và đóng gói điều hòa máy lạnh chuyên nghiệp, đảm bảo an toàn trong suốt quá trình di chuyển.						</t>
+  </si>
+  <si>
+    <t>Tháo lắp, đóng gói</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tháo lắp, đóng gói các đồ vật khác		
+150.000đ/bộ cho các đồ vật nhỏ &lt;=5kg		
+300.000đ/bộ cho các đồ vật lớn &gt;6kg		</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phí: 150.000đ/bộ cho các đồ vật nhỏ &lt;=5kg, 300.000đ/bộ cho các đồ vật lớn &gt;6kg.					
+Bao gồm: Dịch vụ tháo lắp và đóng gói các đồ vật khác như tủ, kệ, đồ điện tử, đảm bảo an toàn khi vận chuyển.					</t>
+  </si>
+  <si>
+    <t>Dịch vụ bảo vệ hàng hóa đặc biệt</t>
+  </si>
+  <si>
+    <t>Giá trị tài sản (VNĐ)</t>
+  </si>
+  <si>
+    <t>Phí dịch vụ bảo vệ (VNĐ)</t>
+  </si>
+  <si>
+    <t>Dưới 50 triệu VNĐ</t>
+  </si>
+  <si>
+    <t>200.000đ</t>
+  </si>
+  <si>
+    <t>Từ 50 triệu - 100 triệu VNĐ</t>
+  </si>
+  <si>
+    <t>300.000đ</t>
+  </si>
+  <si>
+    <t>Từ 100 triệu - 200 triệu VNĐ</t>
+  </si>
+  <si>
+    <t>Trên 200 triệu VNĐ</t>
+  </si>
+  <si>
+    <t>500.000đ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phí chờ 60.000đ/h   </t>
+  </si>
+  <si>
+    <t>system</t>
+  </si>
+  <si>
+    <t>Hỗ trợ tài xế 10.000đ/ng</t>
+  </si>
+  <si>
+    <t>Hỗ trợ bốc vác 10.000đ/ng</t>
+  </si>
+  <si>
+    <t>Chứng từ điện tử 5.000đ</t>
+  </si>
+  <si>
+    <t>Dịch vụ tư vấn phong thủy</t>
+  </si>
+  <si>
+    <t>Phí: 500.000đ/người</t>
+  </si>
+  <si>
+    <t>Thông báo xác nhận đặt đơn thành công</t>
+  </si>
+  <si>
+    <t>Title: Xác nhận đặt đơn</t>
+  </si>
+  <si>
+    <t>Body: Đơn hàng của bạn đã được đặt thành công! Chúng tôi sẽ sắp xếp tài xế và nhân viên bốc vác trong thời gian sớm nhất. Cảm ơn bạn đã tin tưởng sử dụng MoveMate.</t>
+  </si>
+  <si>
+    <t>Thông báo tài xế được gán đơn hàng</t>
+  </si>
+  <si>
+    <t>Title: Đã có tài xế nhận đơn hàng của bạn</t>
+  </si>
+  <si>
+    <t>Body: Tài xế [Tên tài xế] đã được gán để thực hiện đơn hàng của bạn. Bạn có thể theo dõi quá trình vận chuyển trong ứng dụng.</t>
+  </si>
+  <si>
+    <t>Thông báo tài xế đang đến</t>
+  </si>
+  <si>
+    <t>Title: Tài xế đang trên đường đến</t>
+  </si>
+  <si>
+    <t>Body: Tài xế [Tên tài xế] đang di chuyển đến địa chỉ của bạn. Vui lòng chuẩn bị để đón tiếp.</t>
+  </si>
+  <si>
+    <t>Thông báo tài xế đã đến</t>
+  </si>
+  <si>
+    <t>Title: Tài xế đã đến nơi</t>
+  </si>
+  <si>
+    <t>Body: Tài xế [Tên tài xế] đã có mặt tại địa chỉ của bạn. Việc vận chuyển sẽ được bắt đầu ngay khi bạn sẵn sàng.</t>
+  </si>
+  <si>
+    <t>Thông báo sự cố trong quá trình vận chuyển</t>
+  </si>
+  <si>
+    <t>Title: Đã xảy ra sự cố</t>
+  </si>
+  <si>
+    <t>Body: Đã có sự cố xảy ra trong quá trình vận chuyển. Tài xế sẽ liên hệ với bạn để giải quyết và cập nhật thông tin chi tiết.</t>
+  </si>
+  <si>
+    <t>Thông báo đơn hàng hoàn thành</t>
+  </si>
+  <si>
+    <t>Title: Đơn hàng đã hoàn tất</t>
+  </si>
+  <si>
+    <t>Body: Đơn hàng của bạn đã được giao thành công. Cảm ơn bạn đã sử dụng dịch vụ MoveMate. Bạn có thể đánh giá chất lượng dịch vụ ngay trong ứng dụng.</t>
+  </si>
+  <si>
+    <t>Thông báo thay đổi ngày vận chuyển</t>
+  </si>
+  <si>
+    <t>Title: Đã thay đổi ngày vận chuyển</t>
+  </si>
+  <si>
+    <t>Body: Đơn hàng của bạn đã được thay đổi lịch vận chuyển thành [ngày mới]. Nếu bạn có thắc mắc, vui lòng liên hệ với chúng tôi.</t>
+  </si>
+  <si>
+    <t>Thông báo yêu cầu thanh toán</t>
+  </si>
+  <si>
+    <t>Title: Yêu cầu thanh toán</t>
+  </si>
+  <si>
+    <t>Body: Đơn hàng của bạn yêu cầu thanh toán. Vui lòng hoàn tất thanh toán để tiếp tục quá trình vận chuyển.</t>
+  </si>
+  <si>
+    <t>Thông báo hủy đơn hàng</t>
+  </si>
+  <si>
+    <t>Title: Đơn hàng đã bị hủy</t>
+  </si>
+  <si>
+    <t>Body: Đơn hàng của bạn đã bị hủy theo yêu cầu. Nếu bạn muốn đặt lại, vui lòng truy cập ứng dụng để thực hiện.</t>
+  </si>
+  <si>
+    <t>Thông báo đăng ký làm bốc vác thành công</t>
+  </si>
+  <si>
+    <t>Title: Đăng ký làm bốc vác thành công</t>
+  </si>
+  <si>
+    <t>Body: Bạn đã đăng ký thành công làm bốc vác. Hãy chờ thông báo từ hệ thống về các công việc sắp tới.</t>
+  </si>
+  <si>
+    <t>Thông báo đặt lịch review thành công</t>
+  </si>
+  <si>
+    <t>Title: Đặt lịch review thành công</t>
+  </si>
+  <si>
+    <t>Body: Bạn đã đặt lịch cho reviewer đến nhà review thành công. Reviewer sẽ đến vào [ngày/thời gian] để tiến hành đánh giá.</t>
+  </si>
+  <si>
+    <t>Thông báo reviewer đang đến</t>
+  </si>
+  <si>
+    <t>Title: Reviewer đang trên đường đến</t>
+  </si>
+  <si>
+    <t>Body: Reviewer đang di chuyển đến địa chỉ [địa chỉ] và dự kiến sẽ có mặt vào lúc [thời gian]. Vui lòng chuẩn bị để tiếp đón.</t>
+  </si>
+  <si>
+    <t>Thông báo reviewer đã đến</t>
+  </si>
+  <si>
+    <t>Title: Reviewer đã đến nơi</t>
+  </si>
+  <si>
+    <t>Body: Reviewer đã có mặt tại [địa chỉ] và đang tiến hành đánh giá ngôi nhà của bạn.</t>
+  </si>
+  <si>
+    <t>Thông báo hoàn thành đánh giá nhà</t>
+  </si>
+  <si>
+    <t>Title: Hoàn thành đánh giá nhà</t>
+  </si>
+  <si>
+    <t>Body: Quá trình review nhà của bạn đã hoàn tất. Reviewer đã cung cấp đầy đủ thông tin và nhận xét về quá trình chuyển nhà. Bạn có thể tiến hành bước tiếp theo.</t>
+  </si>
+  <si>
+    <t>Thông báo cần cung cấp thêm thông tin trước khi review</t>
+  </si>
+  <si>
+    <t>Title: Cung cấp thêm thông tin cho review</t>
+  </si>
+  <si>
+    <t>Body: Vui lòng cung cấp thêm thông tin chi tiết về ngôi nhà (như kích thước, số tầng, tình trạng vật dụng) để reviewer có thể đánh giá chính xác.</t>
+  </si>
+  <si>
+    <t>Thông báo thay đổi lịch review</t>
+  </si>
+  <si>
+    <t>Title: Lịch review đã thay đổi</t>
+  </si>
+  <si>
+    <t>Body: Lịch review của bạn đã được điều chỉnh. Reviewer sẽ đến vào [ngày/thời gian mới]. Vui lòng xác nhận lại thông tin.</t>
+  </si>
+  <si>
+    <t>Thông báo hủy lịch review</t>
+  </si>
+  <si>
+    <t>Title: Lịch review đã bị hủy</t>
+  </si>
+  <si>
+    <t>Body: Lịch review tại [địa chỉ] đã bị hủy. Vui lòng liên hệ với chúng tôi để đặt lại lịch nếu cần.</t>
+  </si>
+  <si>
+    <t>Thông báo yêu cầu đánh giá reviewer</t>
+  </si>
+  <si>
+    <t>Title: Đánh giá reviewer</t>
+  </si>
+  <si>
+    <t>Body: Quá trình review nhà của bạn đã hoàn tất. Vui lòng đánh giá chất lượng dịch vụ của reviewer để chúng tôi có thể cải thiện dịch vụ tốt hơn.</t>
+  </si>
+  <si>
+    <t>Thông báo cần thay đổi thông tin nhà</t>
+  </si>
+  <si>
+    <t>Title: Cập nhật thông tin nhà cho review</t>
+  </si>
+  <si>
+    <t>Body: Vui lòng kiểm tra và cập nhật lại thông tin nhà nếu có thay đổi để reviewer có thể tiến hành đánh giá chính xác hơn.</t>
+  </si>
+  <si>
+    <t>Thông báo vấn đề khi review</t>
   </si>
 </sst>
 </file>
@@ -3080,7 +3196,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d-m"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -3212,8 +3328,13 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Docs-Calibri"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3244,8 +3365,14 @@
         <bgColor rgb="FF00FFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="29">
+  <borders count="32">
     <border/>
     <border>
       <left/>
@@ -3559,11 +3686,41 @@
         <color rgb="FF284E3F"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="124">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
@@ -3868,9 +4025,72 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="29" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="30" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf quotePrefix="1" borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="31" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="29" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="2" fillId="6" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3938,7 +4158,7 @@
     <xdr:ext cx="876300" cy="676275"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png"/>
+        <xdr:cNvPr id="0" name="image4.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3966,7 +4186,7 @@
     <xdr:ext cx="876300" cy="723900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png"/>
+        <xdr:cNvPr id="0" name="image1.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3994,7 +4214,7 @@
     <xdr:ext cx="923925" cy="771525"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image4.png"/>
+        <xdr:cNvPr id="0" name="image2.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4022,7 +4242,7 @@
     <xdr:ext cx="5391150" cy="771525"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4050,7 +4270,7 @@
     <xdr:ext cx="5238750" cy="676275"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4115,7 +4335,7 @@
     <xdr:ext cx="3124200" cy="2686050"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image9.png"/>
+        <xdr:cNvPr id="0" name="image10.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4143,7 +4363,7 @@
     <xdr:ext cx="4114800" cy="2552700"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image7.png"/>
+        <xdr:cNvPr id="0" name="image9.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4171,7 +4391,7 @@
     <xdr:ext cx="4581525" cy="2276475"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image10.png"/>
+        <xdr:cNvPr id="0" name="image6.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4199,7 +4419,7 @@
     <xdr:ext cx="3733800" cy="2619375"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.png"/>
+        <xdr:cNvPr id="0" name="image7.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5735,216 +5955,493 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1"/>
-    <row r="2" ht="14.25" customHeight="1"/>
+    <row r="2" ht="14.25" customHeight="1">
+      <c r="B2" s="3" t="s">
+        <v>508</v>
+      </c>
+    </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="B3" s="1" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25" customHeight="1"/>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" ht="14.25" customHeight="1">
+      <c r="B4" s="3" t="s">
+        <v>509</v>
+      </c>
+    </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="B5" s="4" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="6" ht="14.25" customHeight="1"/>
+      <c r="B5" s="123" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25" customHeight="1">
+      <c r="B6" s="3" t="s">
+        <v>511</v>
+      </c>
+    </row>
     <row r="7" ht="14.25" customHeight="1"/>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="B8" s="6" t="s">
-        <v>450</v>
+      <c r="B8" s="59" t="s">
+        <v>512</v>
       </c>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="B9" s="59" t="s">
-        <v>451</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="10" ht="14.25" customHeight="1"/>
+        <v>513</v>
+      </c>
+    </row>
+    <row r="10" ht="14.25" customHeight="1">
+      <c r="B10" s="3" t="s">
+        <v>514</v>
+      </c>
+    </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="B11" s="4" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="12" ht="14.25" customHeight="1"/>
-    <row r="13" ht="14.25" customHeight="1"/>
+      <c r="B11" s="4"/>
+    </row>
+    <row r="12" ht="14.25" customHeight="1">
+      <c r="B12" s="3" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="13" ht="14.25" customHeight="1">
+      <c r="B13" s="3" t="s">
+        <v>516</v>
+      </c>
+    </row>
     <row r="14" ht="14.25" customHeight="1">
-      <c r="B14" s="6" t="s">
-        <v>454</v>
+      <c r="B14" s="59" t="s">
+        <v>517</v>
       </c>
     </row>
     <row r="15" ht="14.25" customHeight="1">
-      <c r="B15" s="6" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="16" ht="14.25" customHeight="1"/>
+      <c r="B15" s="6"/>
+    </row>
+    <row r="16" ht="14.25" customHeight="1">
+      <c r="B16" s="3" t="s">
+        <v>518</v>
+      </c>
+    </row>
     <row r="17" ht="14.25" customHeight="1">
-      <c r="B17" s="4" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="18" ht="14.25" customHeight="1"/>
+      <c r="B17" s="123" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="18" ht="14.25" customHeight="1">
+      <c r="B18" s="3" t="s">
+        <v>520</v>
+      </c>
+    </row>
     <row r="19" ht="14.25" customHeight="1"/>
     <row r="20" ht="14.25" customHeight="1">
-      <c r="B20" s="6" t="s">
-        <v>457</v>
+      <c r="B20" s="59" t="s">
+        <v>521</v>
       </c>
     </row>
     <row r="21" ht="14.25" customHeight="1">
-      <c r="B21" s="6" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="22" ht="14.25" customHeight="1"/>
+      <c r="B21" s="59" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="22" ht="14.25" customHeight="1">
+      <c r="B22" s="3" t="s">
+        <v>523</v>
+      </c>
+    </row>
     <row r="23" ht="14.25" customHeight="1">
-      <c r="B23" s="4" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
+      <c r="B23" s="4"/>
+    </row>
+    <row r="24" ht="14.25" customHeight="1">
+      <c r="B24" s="3" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="25" ht="14.25" customHeight="1">
+      <c r="B25" s="3" t="s">
+        <v>525</v>
+      </c>
+    </row>
     <row r="26" ht="14.25" customHeight="1">
-      <c r="B26" s="6" t="s">
-        <v>459</v>
+      <c r="B26" s="59" t="s">
+        <v>526</v>
       </c>
     </row>
     <row r="27" ht="14.25" customHeight="1">
-      <c r="B27" s="6" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="28" ht="14.25" customHeight="1"/>
+      <c r="B27" s="6"/>
+    </row>
+    <row r="28" ht="14.25" customHeight="1">
+      <c r="B28" s="3" t="s">
+        <v>527</v>
+      </c>
+    </row>
     <row r="29" ht="14.25" customHeight="1">
-      <c r="B29" s="4" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="30" ht="14.25" customHeight="1"/>
+      <c r="B29" s="123" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="30" ht="14.25" customHeight="1">
+      <c r="B30" s="3" t="s">
+        <v>529</v>
+      </c>
+    </row>
     <row r="31" ht="14.25" customHeight="1"/>
     <row r="32" ht="14.25" customHeight="1">
-      <c r="B32" s="6" t="s">
-        <v>462</v>
+      <c r="B32" s="59" t="s">
+        <v>530</v>
       </c>
     </row>
     <row r="33" ht="14.25" customHeight="1">
-      <c r="B33" s="6" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="34" ht="14.25" customHeight="1"/>
+      <c r="B33" s="59" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="34" ht="14.25" customHeight="1">
+      <c r="B34" s="3" t="s">
+        <v>532</v>
+      </c>
+    </row>
     <row r="35" ht="14.25" customHeight="1">
-      <c r="B35" s="4" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
+      <c r="B35" s="4"/>
+    </row>
+    <row r="36" ht="14.25" customHeight="1">
+      <c r="B36" s="3" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="37" ht="14.25" customHeight="1">
+      <c r="B37" s="3" t="s">
+        <v>534</v>
+      </c>
+    </row>
     <row r="38" ht="14.25" customHeight="1">
-      <c r="B38" s="6" t="s">
-        <v>465</v>
+      <c r="B38" s="59" t="s">
+        <v>535</v>
       </c>
     </row>
     <row r="39" ht="14.25" customHeight="1">
-      <c r="B39" s="6" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="40" ht="14.25" customHeight="1"/>
+      <c r="B39" s="6"/>
+    </row>
+    <row r="40" ht="14.25" customHeight="1">
+      <c r="B40" s="3" t="s">
+        <v>536</v>
+      </c>
+    </row>
     <row r="41" ht="14.25" customHeight="1">
-      <c r="B41" s="4" t="s">
-        <v>467</v>
+      <c r="B41" s="123" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
+    <row r="43" ht="14.25" customHeight="1">
+      <c r="B43" s="3" t="s">
+        <v>508</v>
+      </c>
+    </row>
     <row r="44" ht="14.25" customHeight="1">
-      <c r="B44" s="6" t="s">
-        <v>468</v>
-      </c>
+      <c r="B44" s="6"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
-      <c r="B45" s="6" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
+      <c r="B45" s="59" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="46" ht="14.25" customHeight="1">
+      <c r="B46" s="3" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="47" ht="14.25" customHeight="1">
+      <c r="B47" s="3" t="s">
+        <v>511</v>
+      </c>
+    </row>
     <row r="48" ht="14.25" customHeight="1"/>
-    <row r="49" ht="14.25" customHeight="1"/>
-    <row r="50" ht="14.25" customHeight="1"/>
-    <row r="51" ht="14.25" customHeight="1"/>
+    <row r="49" ht="14.25" customHeight="1">
+      <c r="B49" s="3" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="50" ht="14.25" customHeight="1">
+      <c r="B50" s="3" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="51" ht="14.25" customHeight="1">
+      <c r="B51" s="3" t="s">
+        <v>514</v>
+      </c>
+    </row>
     <row r="52" ht="14.25" customHeight="1"/>
-    <row r="53" ht="14.25" customHeight="1"/>
-    <row r="54" ht="14.25" customHeight="1"/>
-    <row r="55" ht="14.25" customHeight="1"/>
+    <row r="53" ht="14.25" customHeight="1">
+      <c r="B53" s="3" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="54" ht="14.25" customHeight="1">
+      <c r="B54" s="3" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="55" ht="14.25" customHeight="1">
+      <c r="B55" s="3" t="s">
+        <v>517</v>
+      </c>
+    </row>
     <row r="56" ht="14.25" customHeight="1"/>
-    <row r="57" ht="14.25" customHeight="1"/>
-    <row r="58" ht="14.25" customHeight="1"/>
-    <row r="59" ht="14.25" customHeight="1"/>
+    <row r="57" ht="14.25" customHeight="1">
+      <c r="B57" s="3" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="58" ht="14.25" customHeight="1">
+      <c r="B58" s="3" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="59" ht="14.25" customHeight="1">
+      <c r="B59" s="3" t="s">
+        <v>520</v>
+      </c>
+    </row>
     <row r="60" ht="14.25" customHeight="1"/>
-    <row r="61" ht="14.25" customHeight="1"/>
-    <row r="62" ht="14.25" customHeight="1"/>
-    <row r="63" ht="14.25" customHeight="1"/>
+    <row r="61" ht="14.25" customHeight="1">
+      <c r="B61" s="3" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="62" ht="14.25" customHeight="1">
+      <c r="B62" s="3" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="63" ht="14.25" customHeight="1">
+      <c r="B63" s="3" t="s">
+        <v>523</v>
+      </c>
+    </row>
     <row r="64" ht="14.25" customHeight="1"/>
-    <row r="65" ht="14.25" customHeight="1"/>
-    <row r="66" ht="14.25" customHeight="1"/>
-    <row r="67" ht="14.25" customHeight="1"/>
+    <row r="65" ht="14.25" customHeight="1">
+      <c r="B65" s="3" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="66" ht="14.25" customHeight="1">
+      <c r="B66" s="3" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="67" ht="14.25" customHeight="1">
+      <c r="B67" s="3" t="s">
+        <v>526</v>
+      </c>
+    </row>
     <row r="68" ht="14.25" customHeight="1"/>
-    <row r="69" ht="14.25" customHeight="1"/>
-    <row r="70" ht="14.25" customHeight="1"/>
-    <row r="71" ht="14.25" customHeight="1"/>
+    <row r="69" ht="14.25" customHeight="1">
+      <c r="B69" s="3" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="70" ht="14.25" customHeight="1">
+      <c r="B70" s="3" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="71" ht="14.25" customHeight="1">
+      <c r="B71" s="3" t="s">
+        <v>529</v>
+      </c>
+    </row>
     <row r="72" ht="14.25" customHeight="1"/>
-    <row r="73" ht="14.25" customHeight="1"/>
-    <row r="74" ht="14.25" customHeight="1"/>
-    <row r="75" ht="14.25" customHeight="1"/>
+    <row r="73" ht="14.25" customHeight="1">
+      <c r="B73" s="3" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="74" ht="14.25" customHeight="1">
+      <c r="B74" s="3" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="75" ht="14.25" customHeight="1">
+      <c r="B75" s="3" t="s">
+        <v>532</v>
+      </c>
+    </row>
     <row r="76" ht="14.25" customHeight="1"/>
-    <row r="77" ht="14.25" customHeight="1"/>
-    <row r="78" ht="14.25" customHeight="1"/>
-    <row r="79" ht="14.25" customHeight="1"/>
+    <row r="77" ht="14.25" customHeight="1">
+      <c r="B77" s="3" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="78" ht="14.25" customHeight="1">
+      <c r="B78" s="3" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="79" ht="14.25" customHeight="1">
+      <c r="B79" s="3" t="s">
+        <v>535</v>
+      </c>
+    </row>
     <row r="80" ht="14.25" customHeight="1"/>
-    <row r="81" ht="14.25" customHeight="1"/>
-    <row r="82" ht="14.25" customHeight="1"/>
+    <row r="81" ht="14.25" customHeight="1">
+      <c r="B81" s="3" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="82" ht="14.25" customHeight="1">
+      <c r="B82" s="3" t="s">
+        <v>537</v>
+      </c>
+    </row>
     <row r="83" ht="14.25" customHeight="1"/>
-    <row r="84" ht="14.25" customHeight="1"/>
+    <row r="84" ht="14.25" customHeight="1">
+      <c r="B84" s="3" t="s">
+        <v>538</v>
+      </c>
+    </row>
     <row r="85" ht="14.25" customHeight="1"/>
-    <row r="86" ht="14.25" customHeight="1"/>
-    <row r="87" ht="14.25" customHeight="1"/>
-    <row r="88" ht="14.25" customHeight="1"/>
+    <row r="86" ht="14.25" customHeight="1">
+      <c r="B86" s="3" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="87" ht="14.25" customHeight="1">
+      <c r="B87" s="3" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="88" ht="14.25" customHeight="1">
+      <c r="B88" s="3" t="s">
+        <v>541</v>
+      </c>
+    </row>
     <row r="89" ht="14.25" customHeight="1"/>
-    <row r="90" ht="14.25" customHeight="1"/>
-    <row r="91" ht="14.25" customHeight="1"/>
-    <row r="92" ht="14.25" customHeight="1"/>
+    <row r="90" ht="14.25" customHeight="1">
+      <c r="B90" s="3" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="91" ht="14.25" customHeight="1">
+      <c r="B91" s="3" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="92" ht="14.25" customHeight="1">
+      <c r="B92" s="3" t="s">
+        <v>544</v>
+      </c>
+    </row>
     <row r="93" ht="14.25" customHeight="1"/>
-    <row r="94" ht="14.25" customHeight="1"/>
-    <row r="95" ht="14.25" customHeight="1"/>
-    <row r="96" ht="14.25" customHeight="1"/>
+    <row r="94" ht="14.25" customHeight="1">
+      <c r="B94" s="3" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="95" ht="14.25" customHeight="1">
+      <c r="B95" s="3" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="96" ht="14.25" customHeight="1">
+      <c r="B96" s="3" t="s">
+        <v>547</v>
+      </c>
+    </row>
     <row r="97" ht="14.25" customHeight="1"/>
-    <row r="98" ht="14.25" customHeight="1"/>
-    <row r="99" ht="14.25" customHeight="1"/>
-    <row r="100" ht="14.25" customHeight="1"/>
+    <row r="98" ht="14.25" customHeight="1">
+      <c r="B98" s="3" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="99" ht="14.25" customHeight="1">
+      <c r="B99" s="3" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="100" ht="14.25" customHeight="1">
+      <c r="B100" s="3" t="s">
+        <v>550</v>
+      </c>
+    </row>
     <row r="101" ht="14.25" customHeight="1"/>
-    <row r="102" ht="14.25" customHeight="1"/>
-    <row r="103" ht="14.25" customHeight="1"/>
-    <row r="104" ht="14.25" customHeight="1"/>
+    <row r="102" ht="14.25" customHeight="1">
+      <c r="B102" s="3" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="103" ht="14.25" customHeight="1">
+      <c r="B103" s="3" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="104" ht="14.25" customHeight="1">
+      <c r="B104" s="3" t="s">
+        <v>553</v>
+      </c>
+    </row>
     <row r="105" ht="14.25" customHeight="1"/>
-    <row r="106" ht="14.25" customHeight="1"/>
-    <row r="107" ht="14.25" customHeight="1"/>
-    <row r="108" ht="14.25" customHeight="1"/>
+    <row r="106" ht="14.25" customHeight="1">
+      <c r="B106" s="3" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="107" ht="14.25" customHeight="1">
+      <c r="B107" s="3" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="108" ht="14.25" customHeight="1">
+      <c r="B108" s="3" t="s">
+        <v>556</v>
+      </c>
+    </row>
     <row r="109" ht="14.25" customHeight="1"/>
-    <row r="110" ht="14.25" customHeight="1"/>
-    <row r="111" ht="14.25" customHeight="1"/>
-    <row r="112" ht="14.25" customHeight="1"/>
+    <row r="110" ht="14.25" customHeight="1">
+      <c r="B110" s="3" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="111" ht="14.25" customHeight="1">
+      <c r="B111" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="112" ht="14.25" customHeight="1">
+      <c r="B112" s="3" t="s">
+        <v>559</v>
+      </c>
+    </row>
     <row r="113" ht="14.25" customHeight="1"/>
-    <row r="114" ht="14.25" customHeight="1"/>
-    <row r="115" ht="14.25" customHeight="1"/>
-    <row r="116" ht="14.25" customHeight="1"/>
+    <row r="114" ht="14.25" customHeight="1">
+      <c r="B114" s="3" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="115" ht="14.25" customHeight="1">
+      <c r="B115" s="3" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="116" ht="14.25" customHeight="1">
+      <c r="B116" s="3" t="s">
+        <v>562</v>
+      </c>
+    </row>
     <row r="117" ht="14.25" customHeight="1"/>
-    <row r="118" ht="14.25" customHeight="1"/>
-    <row r="119" ht="14.25" customHeight="1"/>
-    <row r="120" ht="14.25" customHeight="1"/>
+    <row r="118" ht="14.25" customHeight="1">
+      <c r="B118" s="3" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="119" ht="14.25" customHeight="1">
+      <c r="B119" s="3" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="120" ht="14.25" customHeight="1">
+      <c r="B120" s="3" t="s">
+        <v>565</v>
+      </c>
+    </row>
     <row r="121" ht="14.25" customHeight="1"/>
     <row r="122" ht="14.25" customHeight="1"/>
     <row r="123" ht="14.25" customHeight="1"/>
@@ -42881,101 +43378,102 @@
         <v>398</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>400</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>401</v>
-      </c>
-    </row>
     <row r="11">
       <c r="A11" s="3" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="s">
         <v>402</v>
       </c>
-      <c r="B11" s="3" t="s">
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="s">
         <v>403</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="E12" s="3" t="s">
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="s">
         <v>404</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="E13" s="3" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="E14" s="3" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="3" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="3" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
-        <v>410</v>
+        <v>406</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="s">
         <v>411</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="3" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="3" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="3" t="s">
-        <v>414</v>
-      </c>
+      <c r="A29" s="3"/>
     </row>
     <row r="30">
       <c r="A30" s="3" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" s="3" t="s">
-        <v>416</v>
-      </c>
-    </row>
     <row r="32">
       <c r="A32" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="3" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
     </row>
     <row r="34">
@@ -42985,95 +43483,114 @@
     </row>
     <row r="35">
       <c r="A35" s="3" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="3" t="s">
-        <v>419</v>
+      <c r="A36" s="101"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="3" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="101"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="3" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="3" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="B43" s="3" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="B45" s="3" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" s="3" t="s">
+    <row r="41">
+      <c r="A41" s="3" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" s="56" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="70" t="s">
+    <row r="42">
+      <c r="A42" s="101"/>
+    </row>
+    <row r="49">
+      <c r="B49" s="3" t="s">
         <v>424</v>
       </c>
-      <c r="B48" s="70" t="s">
-        <v>400</v>
-      </c>
-      <c r="C48" s="70" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="C49" s="101" t="s">
+    </row>
+    <row r="51">
+      <c r="B51" s="3" t="s">
         <v>425</v>
       </c>
-      <c r="E49" s="102"/>
-    </row>
-    <row r="50">
-      <c r="E50" s="102"/>
-    </row>
-    <row r="51">
-      <c r="A51" s="56" t="s">
-        <v>426</v>
-      </c>
-      <c r="E51" s="102"/>
     </row>
     <row r="52">
       <c r="A52" s="3" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="56" t="s">
         <v>427</v>
       </c>
-      <c r="B52" s="3" t="s">
-        <v>427</v>
-      </c>
-      <c r="C52" s="3" t="s">
+    </row>
+    <row r="54">
+      <c r="A54" s="70" t="s">
         <v>428</v>
       </c>
-      <c r="E52" s="102"/>
-    </row>
-    <row r="54">
-      <c r="A54" s="3" t="s">
+      <c r="B54" s="70" t="s">
         <v>429</v>
+      </c>
+      <c r="C54" s="70" t="s">
+        <v>430</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="3" t="s">
-        <v>430</v>
-      </c>
+        <v>431</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="C55" s="102" t="s">
+        <v>433</v>
+      </c>
+      <c r="E55" s="103"/>
+    </row>
+    <row r="56">
+      <c r="E56" s="103"/>
     </row>
     <row r="57">
-      <c r="E57" s="3"/>
+      <c r="A57" s="56" t="s">
+        <v>434</v>
+      </c>
+      <c r="E57" s="103"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="E58" s="103"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="3" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="3" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="E63" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -43089,30 +43606,36 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="27.0"/>
+    <col customWidth="1" min="2" max="2" width="22.71"/>
+    <col customWidth="1" min="3" max="4" width="21.86"/>
+    <col customWidth="1" min="10" max="10" width="25.14"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="74" t="s">
-        <v>431</v>
+        <v>439</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="78" t="s">
-        <v>432</v>
+        <v>440</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="78" t="s">
-        <v>433</v>
+        <v>441</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="78" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="78" t="s">
-        <v>435</v>
+        <v>443</v>
       </c>
     </row>
     <row r="6">
@@ -43120,37 +43643,37 @@
     </row>
     <row r="7">
       <c r="A7" s="74" t="s">
-        <v>436</v>
+        <v>444</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="78" t="s">
-        <v>437</v>
+        <v>445</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="78" t="s">
-        <v>438</v>
+        <v>446</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="78" t="s">
-        <v>439</v>
+        <v>447</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="78" t="s">
-        <v>440</v>
+        <v>448</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="78" t="s">
-        <v>441</v>
+        <v>449</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="78" t="s">
-        <v>442</v>
+        <v>450</v>
       </c>
     </row>
     <row r="14">
@@ -43158,30 +43681,537 @@
     </row>
     <row r="15">
       <c r="A15" s="74" t="s">
-        <v>443</v>
+        <v>451</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="78" t="s">
-        <v>444</v>
+        <v>452</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="78" t="s">
-        <v>445</v>
+        <v>453</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="78" t="s">
-        <v>446</v>
+        <v>454</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="78" t="s">
-        <v>447</v>
+        <v>455</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="104" t="s">
+        <v>457</v>
+      </c>
+      <c r="B23" s="16"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="104" t="s">
+        <v>458</v>
+      </c>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="105" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="106" t="s">
+        <v>460</v>
+      </c>
+      <c r="B24" s="21"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="106" t="s">
+        <v>461</v>
+      </c>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="107" t="s">
+        <v>462</v>
+      </c>
+      <c r="O24" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="Q24" s="59" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="24"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="24"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="108"/>
+      <c r="O25" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="Q25" s="109" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="22"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="23"/>
+      <c r="K26" s="110"/>
+      <c r="O26" s="3" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="106" t="s">
+        <v>468</v>
+      </c>
+      <c r="B27" s="21"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="106" t="s">
+        <v>469</v>
+      </c>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="107" t="s">
+        <v>462</v>
+      </c>
+      <c r="O27" s="3" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="24"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="24"/>
+      <c r="J28" s="25"/>
+      <c r="K28" s="108"/>
+      <c r="O28" s="3" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="22"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="110"/>
+      <c r="O29" s="3" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="106" t="s">
+        <v>473</v>
+      </c>
+      <c r="B30" s="21"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="106" t="s">
+        <v>474</v>
+      </c>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="107" t="s">
+        <v>462</v>
+      </c>
+      <c r="O30" s="3" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="22"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="23"/>
+      <c r="K31" s="110"/>
+      <c r="O31" s="3" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="106" t="s">
+        <v>477</v>
+      </c>
+      <c r="B32" s="21"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="111" t="s">
+        <v>478</v>
+      </c>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="107" t="s">
+        <v>462</v>
+      </c>
+      <c r="O32" s="3" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="24"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="24"/>
+      <c r="J33" s="25"/>
+      <c r="K33" s="108"/>
+      <c r="O33" s="3" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="24"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="24"/>
+      <c r="J34" s="25"/>
+      <c r="K34" s="108"/>
+      <c r="O34" s="3" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="22"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="29"/>
+      <c r="J35" s="23"/>
+      <c r="K35" s="110"/>
+      <c r="O35" s="3" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="106" t="s">
+        <v>482</v>
+      </c>
+      <c r="B36" s="21"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="106" t="s">
+        <v>483</v>
+      </c>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="21"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="107" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="24"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="24"/>
+      <c r="J37" s="25"/>
+      <c r="K37" s="108"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="22"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="29"/>
+      <c r="J38" s="23"/>
+      <c r="K38" s="110"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="106" t="s">
+        <v>484</v>
+      </c>
+      <c r="B39" s="21"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="106" t="s">
+        <v>485</v>
+      </c>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="21"/>
+      <c r="J39" s="18"/>
+      <c r="K39" s="107" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="40" ht="30.0" customHeight="1">
+      <c r="A40" s="22"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="29"/>
+      <c r="J40" s="23"/>
+      <c r="K40" s="110"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="106" t="s">
+        <v>486</v>
+      </c>
+      <c r="B41" s="21"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="106" t="s">
+        <v>487</v>
+      </c>
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="21"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="21"/>
+      <c r="J41" s="18"/>
+      <c r="K41" s="112" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="22"/>
+      <c r="B42" s="29"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="29"/>
+      <c r="F42" s="29"/>
+      <c r="G42" s="29"/>
+      <c r="H42" s="29"/>
+      <c r="I42" s="29"/>
+      <c r="J42" s="23"/>
+      <c r="K42" s="110"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="106" t="s">
+        <v>489</v>
+      </c>
+      <c r="B43" s="21"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="106" t="s">
+        <v>490</v>
+      </c>
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="21"/>
+      <c r="H43" s="21"/>
+      <c r="I43" s="21"/>
+      <c r="J43" s="18"/>
+      <c r="K43" s="112" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="24"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="24"/>
+      <c r="J44" s="25"/>
+      <c r="K44" s="108"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="22"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="23"/>
+      <c r="D45" s="22"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="29"/>
+      <c r="G45" s="29"/>
+      <c r="H45" s="29"/>
+      <c r="I45" s="29"/>
+      <c r="J45" s="23"/>
+      <c r="K45" s="110"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="106" t="s">
+        <v>491</v>
+      </c>
+      <c r="B46" s="113"/>
+      <c r="K46" s="112" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="114" t="s">
+        <v>492</v>
+      </c>
+      <c r="B47" s="115" t="s">
+        <v>493</v>
+      </c>
+      <c r="K47" s="108"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="116" t="s">
+        <v>494</v>
+      </c>
+      <c r="B48" s="117" t="s">
+        <v>495</v>
+      </c>
+      <c r="K48" s="108"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="116" t="s">
+        <v>496</v>
+      </c>
+      <c r="B49" s="117" t="s">
+        <v>497</v>
+      </c>
+      <c r="K49" s="108"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="116" t="s">
+        <v>498</v>
+      </c>
+      <c r="B50" s="117" t="s">
+        <v>273</v>
+      </c>
+      <c r="K50" s="108"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="118" t="s">
+        <v>499</v>
+      </c>
+      <c r="B51" s="119" t="s">
+        <v>500</v>
+      </c>
+      <c r="K51" s="110"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="118" t="s">
+        <v>501</v>
+      </c>
+      <c r="B52" s="23"/>
+      <c r="K52" s="120" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="121" t="s">
+        <v>503</v>
+      </c>
+      <c r="B53" s="13"/>
+      <c r="K53" s="120" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="122" t="s">
+        <v>504</v>
+      </c>
+      <c r="B54" s="13"/>
+      <c r="K54" s="120" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="122" t="s">
+        <v>505</v>
+      </c>
+      <c r="B55" s="13"/>
+      <c r="K55" s="120" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="122" t="s">
+        <v>506</v>
+      </c>
+      <c r="B56" s="13"/>
+      <c r="D56" s="122" t="s">
+        <v>507</v>
+      </c>
+      <c r="E56" s="16"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="16"/>
+      <c r="I56" s="16"/>
+      <c r="J56" s="13"/>
+      <c r="K56" s="120" t="s">
+        <v>502</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="33">
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A36:C38"/>
+    <mergeCell ref="A39:C40"/>
+    <mergeCell ref="A41:C42"/>
+    <mergeCell ref="A43:C45"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="K24:K26"/>
+    <mergeCell ref="K27:K29"/>
+    <mergeCell ref="K30:K31"/>
+    <mergeCell ref="K32:K35"/>
+    <mergeCell ref="K36:K38"/>
+    <mergeCell ref="K39:K40"/>
+    <mergeCell ref="K41:K42"/>
+    <mergeCell ref="K43:K45"/>
+    <mergeCell ref="K46:K51"/>
+    <mergeCell ref="A32:C35"/>
+    <mergeCell ref="D32:J35"/>
+    <mergeCell ref="D39:J40"/>
+    <mergeCell ref="D41:J42"/>
+    <mergeCell ref="D43:J45"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="D23:J23"/>
+    <mergeCell ref="D24:J26"/>
+    <mergeCell ref="D27:J29"/>
+    <mergeCell ref="A24:C26"/>
+    <mergeCell ref="A27:C29"/>
+    <mergeCell ref="D30:J31"/>
+    <mergeCell ref="A30:C31"/>
+    <mergeCell ref="D36:J38"/>
+    <mergeCell ref="D56:J56"/>
+  </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
chore: update spec do an
</commit_message>
<xml_diff>
--- a/Report/do an.xlsx
+++ b/Report/do an.xlsx
@@ -13,6 +13,7 @@
     <sheet state="visible" name="Sheet3" sheetId="8" r:id="rId11"/>
     <sheet state="visible" name="Sheet4" sheetId="9" r:id="rId12"/>
     <sheet state="visible" name="msg" sheetId="10" r:id="rId13"/>
+    <sheet state="visible" name="rule chọn tài xế" sheetId="11" r:id="rId14"/>
   </sheets>
   <definedNames>
     <definedName hidden="1" localSheetId="6" name="_xlnm._FilterDatabase">Estimate!$A$1:$E$32</definedName>
@@ -20,14 +21,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId14" roundtripDataChecksum="V6SNANVit/Q3hY9fEi5KzOUlYY9DTk4W/VD50w2rCoM="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId15" roundtripDataChecksum="T/0uoDppQati9Udzk42db0fg1Cco7gSdZ8+64lsCClY="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="588">
   <si>
     <t>Nhập: số tầng, loại nhà, diện tích và số phòng</t>
   </si>
@@ -3187,6 +3188,72 @@
   </si>
   <si>
     <t>Thông báo vấn đề khi review</t>
+  </si>
+  <si>
+    <t>Quy Tắc Chọn Tài Xế Cho Booking</t>
+  </si>
+  <si>
+    <t>1. Tiêu Chí Khoảng Cách Gần Nhất</t>
+  </si>
+  <si>
+    <t>Xác định vị trí hiện tại của tài xế: Dựa vào hệ thống GPS tích hợp, hệ thống sẽ lấy vị trí hiện tại của các tài xế có sẵn.</t>
+  </si>
+  <si>
+    <t>Đo khoảng cách từ vị trí tài xế đến vị trí của booking mới: Sử dụng Google Maps API hoặc một công cụ tương tự để tính toán khoảng cách chính xác (theo đường đi) từ vị trí tài xế đến vị trí khách hàng yêu cầu.</t>
+  </si>
+  <si>
+    <t>Lựa chọn tài xế gần nhất: Ưu tiên tài xế có khoảng cách ngắn nhất đến vị trí khách hàng tại thời điểm hiện tại.</t>
+  </si>
+  <si>
+    <t>2. Tiêu Chí Thời Gian Rảnh Sắp Tới</t>
+  </si>
+  <si>
+    <t>Xác định thời gian kết thúc booking trước đó của tài xế: Hệ thống theo dõi lịch làm việc của tài xế và biết được thời gian kết thúc của booking hiện tại hoặc booking gần nhất mà tài xế thực hiện.</t>
+  </si>
+  <si>
+    <t>Dự đoán thời gian rảnh: Dựa trên thời gian kết thúc dự kiến của booking hiện tại (hoặc gần nhất), hệ thống tính toán thời gian rảnh sắp tới của tài xế, tức là khoảng thời gian mà tài xế có thể nhận thêm booking mới.</t>
+  </si>
+  <si>
+    <t>Kiểm tra xem tài xế có rảnh không: Tài xế chỉ có thể được chọn nếu thời gian rảnh của họ khớp với yêu cầu thời gian booking mới của khách hàng.</t>
+  </si>
+  <si>
+    <t>4. Quy Trình Chọn Tài Xế Cho Booking Mới:</t>
+  </si>
+  <si>
+    <t>Bước 1: Hệ thống xác định danh sách các tài xế sẵn sàng nhận cuốc và đo khoảng cách từ vị trí của họ đến vị trí booking mới.</t>
+  </si>
+  <si>
+    <t>Bước 2: Lọc danh sách tài xế theo khoảng cách gần nhất.</t>
+  </si>
+  <si>
+    <t>hoặc nếu không có tài xế đang rảnh</t>
+  </si>
+  <si>
+    <t>Bước 1: Kiểm tra thời gian rảnh sắp tới của tài xế, dựa trên thời gian kết thúc booking trước đó.</t>
+  </si>
+  <si>
+    <t>Bước 2: Chọn tài xế có thời gian rảnh khớp với yêu cầu booking và khoảng cách gần nhất.</t>
+  </si>
+  <si>
+    <t>5. Trường Hợp Đặc Biệt:</t>
+  </si>
+  <si>
+    <t>Nếu không có tài xế nào có khoảng cách gần và thời gian rảnh phù hợp: Hệ thống sẽ hiển thị thông báo yêu cầu khách hàng chờ thêm 30p hoặc đề xuất thời gian rảnh tiếp theo của tài xế gần nhất.</t>
+  </si>
+  <si>
+    <t>ƯỚC LƯỢNG THỜI GIAN HOÀN THÀNH 1 BOOKING</t>
+  </si>
+  <si>
+    <t>Ước lượng thời gian hoàn thành công việc: Hệ thống có thể ước tính thời gian hoàn thành dựa trên:</t>
+  </si>
+  <si>
+    <t>Khoảng cách di chuyển: Sử dụng bản đồ và khoảng cách giữa điểm nhận và điểm giao hàng.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Khối lượng công việc: Dựa trên thời gian thực mà tài xế và bốc vác cập nhật status, thời gian bốc dỡ </t>
+  </si>
+  <si>
+    <t>Tính thời gian kết thúc dự kiến: Dựa trên thời gian bắt đầu và ước lượng thời gian hoàn thành, hệ thống có thể tính toán được thời gian tài xế sẽ kết thúc công việc hiện tại.</t>
   </si>
 </sst>
 </file>
@@ -4158,7 +4225,7 @@
     <xdr:ext cx="876300" cy="676275"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image4.png"/>
+        <xdr:cNvPr id="0" name="image3.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4242,7 +4309,7 @@
     <xdr:ext cx="5391150" cy="771525"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image4.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4270,7 +4337,7 @@
     <xdr:ext cx="5238750" cy="676275"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4295,6 +4362,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
   <xdr:oneCellAnchor>
@@ -4307,7 +4378,7 @@
     <xdr:ext cx="4171950" cy="2686050"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image8.png"/>
+        <xdr:cNvPr id="0" name="image6.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4363,7 +4434,7 @@
     <xdr:ext cx="4114800" cy="2552700"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image9.png"/>
+        <xdr:cNvPr id="0" name="image8.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4391,7 +4462,7 @@
     <xdr:ext cx="4581525" cy="2276475"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.png"/>
+        <xdr:cNvPr id="0" name="image9.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -7326,6 +7397,132 @@
   <printOptions/>
   <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>
   <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="2">
+      <c r="B2" s="74" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="56" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="3" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="3" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="3" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="56" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="3" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="3" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="3" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="56" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="3" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="3" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="14" ht="22.5" customHeight="1">
+      <c r="A14" s="102" t="s">
+        <v>578</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="3" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" s="56" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" s="3" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="C20" s="56" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="C21" s="3" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="C22" s="3" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="C23" s="3" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="C24" s="3" t="s">
+        <v>587</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A14:A15"/>
+  </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -44178,39 +44375,39 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="D23:J23"/>
+    <mergeCell ref="A24:C26"/>
+    <mergeCell ref="D24:J26"/>
+    <mergeCell ref="K24:K26"/>
+    <mergeCell ref="D27:J29"/>
+    <mergeCell ref="K27:K29"/>
+    <mergeCell ref="D39:J40"/>
+    <mergeCell ref="D41:J42"/>
+    <mergeCell ref="K41:K42"/>
+    <mergeCell ref="D43:J45"/>
+    <mergeCell ref="K43:K45"/>
+    <mergeCell ref="K46:K51"/>
+    <mergeCell ref="D30:J31"/>
+    <mergeCell ref="K30:K31"/>
+    <mergeCell ref="D32:J35"/>
+    <mergeCell ref="K32:K35"/>
+    <mergeCell ref="D36:J38"/>
+    <mergeCell ref="K36:K38"/>
+    <mergeCell ref="K39:K40"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
     <mergeCell ref="A55:B55"/>
     <mergeCell ref="A56:B56"/>
+    <mergeCell ref="D56:J56"/>
+    <mergeCell ref="A27:C29"/>
+    <mergeCell ref="A30:C31"/>
+    <mergeCell ref="A32:C35"/>
     <mergeCell ref="A36:C38"/>
     <mergeCell ref="A39:C40"/>
     <mergeCell ref="A41:C42"/>
     <mergeCell ref="A43:C45"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="K24:K26"/>
-    <mergeCell ref="K27:K29"/>
-    <mergeCell ref="K30:K31"/>
-    <mergeCell ref="K32:K35"/>
-    <mergeCell ref="K36:K38"/>
-    <mergeCell ref="K39:K40"/>
-    <mergeCell ref="K41:K42"/>
-    <mergeCell ref="K43:K45"/>
-    <mergeCell ref="K46:K51"/>
-    <mergeCell ref="A32:C35"/>
-    <mergeCell ref="D32:J35"/>
-    <mergeCell ref="D39:J40"/>
-    <mergeCell ref="D41:J42"/>
-    <mergeCell ref="D43:J45"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="D23:J23"/>
-    <mergeCell ref="D24:J26"/>
-    <mergeCell ref="D27:J29"/>
-    <mergeCell ref="A24:C26"/>
-    <mergeCell ref="A27:C29"/>
-    <mergeCell ref="D30:J31"/>
-    <mergeCell ref="A30:C31"/>
-    <mergeCell ref="D36:J38"/>
-    <mergeCell ref="D56:J56"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>